<commit_message>
Séparation du scénario "s'authentifier"
Séparation du scénario "s'authentifier" en "Se connecter" et "s'inscrire". Passage des titres des scénarios au singulier.
</commit_message>
<xml_diff>
--- a/Analyse/Scénarios.xlsx
+++ b/Analyse/Scénarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyprien.Jaquier\Documents\GitHub\Web-Project\Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\GitHub\Web-Project\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D202574F-B462-4A4D-8B75-5D27262626A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>Actions</t>
   </si>
@@ -41,9 +42,6 @@
     <t>Ouvre la page d'inscription</t>
   </si>
   <si>
-    <t>S'authentifier</t>
-  </si>
-  <si>
     <t>Affiche un message d'erreur</t>
   </si>
   <si>
@@ -89,21 +87,12 @@
     <t>Ouvre la page des annonces de l'utilisateurs</t>
   </si>
   <si>
-    <t>Ajouter des annonces</t>
-  </si>
-  <si>
     <t>Click sur le bouton "Modifier"</t>
   </si>
   <si>
     <t>Ouvre la page de modifitcation de l'annonce</t>
   </si>
   <si>
-    <t>Supprimer ses annonces</t>
-  </si>
-  <si>
-    <t>Modifier ses annonces</t>
-  </si>
-  <si>
     <t>Click sur le bouton "supprimer"</t>
   </si>
   <si>
@@ -131,9 +120,6 @@
     <t>Modifie l'annonce</t>
   </si>
   <si>
-    <t>Contacter les annonceurs</t>
-  </si>
-  <si>
     <t>Click sur l'adresse mail</t>
   </si>
   <si>
@@ -171,12 +157,30 @@
   </si>
   <si>
     <t>Ouvre un formulaire qui envera un mail une fois remplis</t>
+  </si>
+  <si>
+    <t>Supprimer une annonce</t>
+  </si>
+  <si>
+    <t>Contacter un annonceur</t>
+  </si>
+  <si>
+    <t>Modifier une annonce</t>
+  </si>
+  <si>
+    <t>S'inscrire</t>
+  </si>
+  <si>
+    <t>Se connecter</t>
+  </si>
+  <si>
+    <t>Ajouter une annonce</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -314,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -343,6 +347,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,11 +629,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,16 +641,19 @@
     <col min="3" max="3" width="50.5703125" customWidth="1"/>
     <col min="4" max="4" width="55.7109375" customWidth="1"/>
     <col min="5" max="5" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.140625" customWidth="1"/>
+    <col min="10" max="10" width="59.42578125" customWidth="1"/>
+    <col min="11" max="11" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="13" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="3:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
@@ -654,504 +664,504 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="5"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="I10" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="I11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="I12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="I13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1" t="s">
+      <c r="I15" s="5"/>
+      <c r="J15" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
+      <c r="K15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+      <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+      <c r="D19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C24" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+      <c r="D28" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
-      <c r="D14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="3:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="3:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="9" t="s">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+      <c r="D29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+      <c r="D30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C35" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="1" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
-      <c r="D23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
-      <c r="D24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
-      <c r="D25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C30" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="15"/>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="9" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C44" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="14"/>
+      <c r="E44" s="15"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D45" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E45" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="5"/>
-      <c r="D34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
-      <c r="D35" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="5"/>
-      <c r="D36" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="2" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="6"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C41" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="6"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="8" t="s">
-        <v>20</v>
+      <c r="D46" s="3"/>
+      <c r="E46" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+      <c r="C47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="C48" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C50" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="15"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" s="3"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C52" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="14"/>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D53" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C52" s="5" t="s">
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="5"/>
+      <c r="D56" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="1" t="s">
+      <c r="D57" s="7"/>
+      <c r="E57" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C54" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="3"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C56" s="3"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-    </row>
-    <row r="58" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C58" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="14"/>
-      <c r="E58" s="15"/>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C59" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="C60" s="3"/>
       <c r="D60" s="3"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C61" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C62" s="5"/>
-      <c r="D62" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C63" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
+      <c r="E60" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C58:E58"/>
+  <mergeCells count="7">
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C52:E52"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C44:E44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>